<commit_message>
minor update to analysis
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/LAOs/results/Equipment list [target].xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/LAOs/results/Equipment list [target].xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/LAOs/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_C596C0831A976CFAF8160B85E34B3B8656804D9A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32CEC7F3-E18A-4515-9ADE-B73BD0E0773C}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_C596C0831A976CFAF8160B85E34B3B8656804D9A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D122612C-3A5D-4B14-9B31-BD9CA17C79AE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="2628" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment list" sheetId="1" r:id="rId1"/>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="B192" sqref="B192"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1023,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="3">
-        <v>88571.270034187328</v>
+        <v>88571.270034187299</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1035,7 +1035,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="3">
-        <v>1180.327482972195</v>
+        <v>1180.32748297219</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4588,47 +4588,47 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="A109:A111"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="A115:A128"/>
+    <mergeCell ref="A129:A134"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A152"/>
+    <mergeCell ref="A153:A156"/>
+    <mergeCell ref="A163:A165"/>
+    <mergeCell ref="A166:A173"/>
+    <mergeCell ref="A181:A182"/>
+    <mergeCell ref="A183:A184"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="A194:A206"/>
+    <mergeCell ref="A207:A208"/>
+    <mergeCell ref="A215:A216"/>
     <mergeCell ref="A254:A256"/>
     <mergeCell ref="A217:A224"/>
     <mergeCell ref="A225:A226"/>
     <mergeCell ref="A233:A234"/>
     <mergeCell ref="A235:A236"/>
     <mergeCell ref="A244:A246"/>
-    <mergeCell ref="A183:A184"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="A194:A206"/>
-    <mergeCell ref="A207:A208"/>
-    <mergeCell ref="A215:A216"/>
-    <mergeCell ref="A146:A152"/>
-    <mergeCell ref="A153:A156"/>
-    <mergeCell ref="A163:A165"/>
-    <mergeCell ref="A166:A173"/>
-    <mergeCell ref="A181:A182"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="A115:A128"/>
-    <mergeCell ref="A129:A134"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="A109:A111"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>